<commit_message>
Add dpt memilih list
</commit_message>
<xml_diff>
--- a/seeds.xlsx
+++ b/seeds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\(SMK RAY)\pilketos_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B7E13A-3240-4594-8D07-D5A81A8E24FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA2B8C0-4A2A-4ECF-B1C8-2E89C7E68EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{9BE8E3CE-297E-4A2B-9F0C-C1FCB1656B2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{9BE8E3CE-297E-4A2B-9F0C-C1FCB1656B2B}"/>
   </bookViews>
   <sheets>
     <sheet name="kelas" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3998" uniqueCount="1543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="1590">
   <si>
     <t>X BDPM</t>
   </si>
@@ -4740,13 +4740,157 @@
   </si>
   <si>
     <t>paslon3.png</t>
+  </si>
+  <si>
+    <t>Drs. Nahrawi, S.Ag.</t>
+  </si>
+  <si>
+    <t>Drs. Ahmad Muhroj</t>
+  </si>
+  <si>
+    <t>Muhamad Mawahib, S.Kom.</t>
+  </si>
+  <si>
+    <t>Mashuri, S.Pd.</t>
+  </si>
+  <si>
+    <t>Digul Sudirman, S.Sos., M.M.</t>
+  </si>
+  <si>
+    <t>Sapto Sudrato, S.Pd.</t>
+  </si>
+  <si>
+    <t>Ajeng Agustina, S.Pd., M.M., Gr.</t>
+  </si>
+  <si>
+    <t>Indayani, S.E.</t>
+  </si>
+  <si>
+    <t>Imam Saefullah, S.Pd.</t>
+  </si>
+  <si>
+    <t>Abu Bakar Pane G. M., S.Pd.I.</t>
+  </si>
+  <si>
+    <t>Drs. Abdul Aziz Rofiq</t>
+  </si>
+  <si>
+    <t>Nata</t>
+  </si>
+  <si>
+    <t>Tuti Maesaroh</t>
+  </si>
+  <si>
+    <t>Hufron Baidlowi</t>
+  </si>
+  <si>
+    <t>Fandi Ahmad Saktianto, S.Kom</t>
+  </si>
+  <si>
+    <t>Djuliati, SE., M.M.</t>
+  </si>
+  <si>
+    <t>Drs. Nuryaman, S.Ag.</t>
+  </si>
+  <si>
+    <t>Tarno, SE., M.M.</t>
+  </si>
+  <si>
+    <t>Drs. Encep Saepudin, M.M.</t>
+  </si>
+  <si>
+    <t>Drs. Amroni Yahya</t>
+  </si>
+  <si>
+    <t>Suprih SRM, S.Si</t>
+  </si>
+  <si>
+    <t>Rini Fathonah, S.P., M.M.</t>
+  </si>
+  <si>
+    <t>Alyn Anjelika, A.Md</t>
+  </si>
+  <si>
+    <t>Sulaeman</t>
+  </si>
+  <si>
+    <t>Herninta Devayanti, SE.I.</t>
+  </si>
+  <si>
+    <t>Ahmad Irfan Sajidin Malik, S.Pd.</t>
+  </si>
+  <si>
+    <t>Eka Azis Hamsiah, S.Pd.</t>
+  </si>
+  <si>
+    <t>Setianingsih, SE, M.M.</t>
+  </si>
+  <si>
+    <t>M. Rahman, LC</t>
+  </si>
+  <si>
+    <t>Endah Finatariani, SE., M.M.</t>
+  </si>
+  <si>
+    <t>Viska Adawiyah, S.Pd</t>
+  </si>
+  <si>
+    <t>Nifta Alfitriana, S.Kom.I</t>
+  </si>
+  <si>
+    <t>Miftah Farid S.Pd.I</t>
+  </si>
+  <si>
+    <t>Siti Chaerul Bariyyah, S.E.</t>
+  </si>
+  <si>
+    <t>Aris Munandar, S.Or</t>
+  </si>
+  <si>
+    <t>Dhias Priliani, S.Pd</t>
+  </si>
+  <si>
+    <t>Rosya Kurniati, S.Pd</t>
+  </si>
+  <si>
+    <t>Abdul Jabbar, S.Kom</t>
+  </si>
+  <si>
+    <t>Iqbal Firmansyah</t>
+  </si>
+  <si>
+    <t>Anisatul Haqimah, M.Pd.</t>
+  </si>
+  <si>
+    <t>Agus Suryo Purwoko, S.Pd</t>
+  </si>
+  <si>
+    <t>Rani Adha , S.Pd</t>
+  </si>
+  <si>
+    <t>Maleh Bari, M.Pd.</t>
+  </si>
+  <si>
+    <t>Dian Kurniasari</t>
+  </si>
+  <si>
+    <t>Jahlul</t>
+  </si>
+  <si>
+    <t>Aziz Muhtadin</t>
+  </si>
+  <si>
+    <t>Tenaga Pendidik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4815,8 +4959,32 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4857,6 +5025,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD965"/>
         <bgColor rgb="FFFFD965"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4925,11 +5099,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5095,12 +5273,110 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{7C6CC6A4-0EE6-4569-B946-42676B2FBFCC}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{91AA01E2-5C54-4C04-8074-2A115BC72F66}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{EFECEE69-616D-45F5-833A-3ADA45D0EB88}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{9E001D1B-239B-4F55-9D5E-5217D40EB868}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{B75A4631-95DA-4B29-8BED-B34FDAE35DEB}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5501,10 +5777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F38427-3F4B-4EE4-9582-E66A6AA4C335}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5682,6 +5958,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1589</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5691,7 +5975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129EE184-3F6C-41D6-8727-508CC18FDA55}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -5771,7 +6055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AC3B97-E5AF-45F0-8907-9E7251E43FE7}">
   <dimension ref="A1:E502"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A331" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11420,11 +11704,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A502">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11433,17 +11717,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837BB0A9-BE26-463F-B3EE-46121700C607}">
-  <dimension ref="A1:K558"/>
+  <dimension ref="A1:K604"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K584" sqref="K584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
@@ -22006,7 +22290,7 @@
         <v>758</v>
       </c>
       <c r="E361" s="47" t="str">
-        <f t="shared" ref="E361:E558" si="10">A361&amp;B361&amp;C361&amp;D361</f>
+        <f t="shared" ref="E361:E557" si="10">A361&amp;B361&amp;C361&amp;D361</f>
         <v>22230110002</v>
       </c>
       <c r="F361" s="49" t="s">
@@ -27719,13 +28003,13 @@
         <v>1532</v>
       </c>
       <c r="E558" s="47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="E558" si="14">A558&amp;B558&amp;C558&amp;D558</f>
         <v>22230210201</v>
       </c>
-      <c r="F558" s="49" t="s">
+      <c r="F558" s="62" t="s">
         <v>1533</v>
       </c>
-      <c r="G558" s="50" t="s">
+      <c r="G558" s="21" t="s">
         <v>802</v>
       </c>
       <c r="H558" s="24">
@@ -27734,24 +28018,674 @@
       </c>
       <c r="K558" s="28"/>
     </row>
+    <row r="559" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E559" s="47">
+        <v>1</v>
+      </c>
+      <c r="F559" s="63" t="s">
+        <v>1543</v>
+      </c>
+      <c r="G559" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H559" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="560" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E560" s="60">
+        <v>2</v>
+      </c>
+      <c r="F560" s="64" t="s">
+        <v>1544</v>
+      </c>
+      <c r="G560" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H560" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="561" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E561" s="60">
+        <v>3</v>
+      </c>
+      <c r="F561" s="64" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G561" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H561" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="562" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E562" s="60">
+        <v>4</v>
+      </c>
+      <c r="F562" s="64" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G562" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H562" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="563" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E563" s="60">
+        <v>5</v>
+      </c>
+      <c r="F563" s="64" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G563" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H563" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="564" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E564" s="60">
+        <v>6</v>
+      </c>
+      <c r="F564" s="64" t="s">
+        <v>1548</v>
+      </c>
+      <c r="G564" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H564" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="565" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E565" s="60">
+        <v>7</v>
+      </c>
+      <c r="F565" s="64" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G565" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H565" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="566" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E566" s="60">
+        <v>8</v>
+      </c>
+      <c r="F566" s="65" t="s">
+        <v>1550</v>
+      </c>
+      <c r="G566" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H566" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="567" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E567" s="60">
+        <v>9</v>
+      </c>
+      <c r="F567" s="65" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G567" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H567" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="568" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E568" s="60">
+        <v>10</v>
+      </c>
+      <c r="F568" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="G568" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H568" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="569" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E569" s="60">
+        <v>11</v>
+      </c>
+      <c r="F569" s="65" t="s">
+        <v>1553</v>
+      </c>
+      <c r="G569" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H569" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="570" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E570" s="60">
+        <v>12</v>
+      </c>
+      <c r="F570" s="64" t="s">
+        <v>1554</v>
+      </c>
+      <c r="G570" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H570" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="571" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E571" s="60">
+        <v>13</v>
+      </c>
+      <c r="F571" s="64" t="s">
+        <v>1555</v>
+      </c>
+      <c r="G571" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H571" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="572" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E572" s="60">
+        <v>14</v>
+      </c>
+      <c r="F572" s="64" t="s">
+        <v>1556</v>
+      </c>
+      <c r="G572" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H572" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="573" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E573" s="60">
+        <v>15</v>
+      </c>
+      <c r="F573" s="64" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G573" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H573" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="574" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E574" s="60">
+        <v>16</v>
+      </c>
+      <c r="F574" s="64" t="s">
+        <v>1558</v>
+      </c>
+      <c r="G574" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H574" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="575" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E575" s="60">
+        <v>17</v>
+      </c>
+      <c r="F575" s="65" t="s">
+        <v>1559</v>
+      </c>
+      <c r="G575" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H575" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="576" spans="5:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E576" s="60">
+        <v>18</v>
+      </c>
+      <c r="F576" s="66" t="s">
+        <v>1560</v>
+      </c>
+      <c r="G576" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H576" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="577" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E577" s="60">
+        <v>19</v>
+      </c>
+      <c r="F577" s="64" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G577" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H577" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="578" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E578" s="60">
+        <v>20</v>
+      </c>
+      <c r="F578" s="64" t="s">
+        <v>1562</v>
+      </c>
+      <c r="G578" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H578" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="579" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E579" s="60">
+        <v>21</v>
+      </c>
+      <c r="F579" s="64" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G579" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H579" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="580" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E580" s="60">
+        <v>22</v>
+      </c>
+      <c r="F580" s="64" t="s">
+        <v>1564</v>
+      </c>
+      <c r="G580" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H580" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="581" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E581" s="60">
+        <v>23</v>
+      </c>
+      <c r="F581" s="64" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G581" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H581" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="582" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E582" s="60">
+        <v>24</v>
+      </c>
+      <c r="F582" s="67" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G582" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H582" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="583" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E583" s="60">
+        <v>25</v>
+      </c>
+      <c r="F583" s="64" t="s">
+        <v>1567</v>
+      </c>
+      <c r="G583" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H583" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="584" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E584" s="60">
+        <v>26</v>
+      </c>
+      <c r="F584" s="64" t="s">
+        <v>1568</v>
+      </c>
+      <c r="G584" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H584" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="585" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E585" s="60">
+        <v>27</v>
+      </c>
+      <c r="F585" s="65" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G585" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H585" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="586" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E586" s="60">
+        <v>28</v>
+      </c>
+      <c r="F586" s="65" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G586" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H586" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="587" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E587" s="60">
+        <v>29</v>
+      </c>
+      <c r="F587" s="64" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G587" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H587" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="588" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E588" s="60">
+        <v>30</v>
+      </c>
+      <c r="F588" s="64" t="s">
+        <v>1572</v>
+      </c>
+      <c r="G588" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H588" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="589" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E589" s="60">
+        <v>31</v>
+      </c>
+      <c r="F589" s="64" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G589" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H589" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="590" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E590" s="60">
+        <v>32</v>
+      </c>
+      <c r="F590" s="65" t="s">
+        <v>1574</v>
+      </c>
+      <c r="G590" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H590" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="591" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E591" s="60">
+        <v>33</v>
+      </c>
+      <c r="F591" s="65" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G591" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H591" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="592" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E592" s="60">
+        <v>34</v>
+      </c>
+      <c r="F592" s="68" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G592" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H592" s="24">
+        <v>21</v>
+      </c>
+      <c r="J592" s="59"/>
+    </row>
+    <row r="593" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E593" s="60">
+        <v>35</v>
+      </c>
+      <c r="F593" s="68" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G593" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H593" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="594" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E594" s="60">
+        <v>36</v>
+      </c>
+      <c r="F594" s="68" t="s">
+        <v>1578</v>
+      </c>
+      <c r="G594" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H594" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="595" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E595" s="60">
+        <v>37</v>
+      </c>
+      <c r="F595" s="68" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G595" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H595" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="596" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E596" s="60">
+        <v>38</v>
+      </c>
+      <c r="F596" s="68" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G596" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H596" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="597" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E597" s="60">
+        <v>39</v>
+      </c>
+      <c r="F597" s="68" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G597" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H597" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="598" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E598" s="60">
+        <v>40</v>
+      </c>
+      <c r="F598" s="65" t="s">
+        <v>1582</v>
+      </c>
+      <c r="G598" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H598" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="599" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E599" s="60">
+        <v>41</v>
+      </c>
+      <c r="F599" s="68" t="s">
+        <v>1583</v>
+      </c>
+      <c r="G599" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H599" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="600" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E600" s="60">
+        <v>42</v>
+      </c>
+      <c r="F600" s="69" t="s">
+        <v>1584</v>
+      </c>
+      <c r="G600" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H600" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="601" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E601" s="60">
+        <v>43</v>
+      </c>
+      <c r="F601" s="68" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G601" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H601" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="602" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E602" s="60">
+        <v>44</v>
+      </c>
+      <c r="F602" s="68" t="s">
+        <v>1586</v>
+      </c>
+      <c r="G602" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H602" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="603" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E603" s="60">
+        <v>45</v>
+      </c>
+      <c r="F603" s="68" t="s">
+        <v>1587</v>
+      </c>
+      <c r="G603" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H603" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="604" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D604" s="59"/>
+      <c r="E604" s="60">
+        <v>46</v>
+      </c>
+      <c r="F604" s="70" t="s">
+        <v>1588</v>
+      </c>
+      <c r="G604" s="61" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H604" s="24">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D180">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D181:D359">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:E113 E2:E105">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E114:E180 E106">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E181:E359">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E558">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>